<commit_message>
Make Database Window with it's tabs
</commit_message>
<xml_diff>
--- a/Accountant Part time appointments.xlsx
+++ b/Accountant Part time appointments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main Files\SW Work\مصنع حسن سليم للمنتجات البلاستيكية system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB44DACF-9E4F-4712-A5A5-35EF94123012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F7156-54BD-4EDC-BE17-C59D55F4DFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>From</t>
   </si>
@@ -60,8 +60,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,13 +98,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -112,16 +113,17 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="h:mm;@"/>
+      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -147,16 +149,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2ACCAF8-B411-4852-9C2C-3FD66F7A1AE7}" name="Table1" displayName="Table1" ref="A1:E2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E2" xr:uid="{E2ACCAF8-B411-4852-9C2C-3FD66F7A1AE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2ACCAF8-B411-4852-9C2C-3FD66F7A1AE7}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E4" xr:uid="{E2ACCAF8-B411-4852-9C2C-3FD66F7A1AE7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{223B5709-3A1D-4958-AD14-239602AB1970}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{9819534C-24DF-42E3-8032-C6942B255EAA}" name="From" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{38281F84-79DA-49D6-BDA1-B649A01580AB}" name="To" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0EE33BBF-6F5C-4F32-BA15-31AF3428E1FE}" name="Duarations" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{223B5709-3A1D-4958-AD14-239602AB1970}" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9819534C-24DF-42E3-8032-C6942B255EAA}" name="From" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{38281F84-79DA-49D6-BDA1-B649A01580AB}" name="To" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0EE33BBF-6F5C-4F32-BA15-31AF3428E1FE}" name="Duarations" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[To]]-Table1[[#This Row],[From]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7251073A-ECCC-4632-998C-485EFAF1F130}" name="offline / online" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7251073A-ECCC-4632-998C-485EFAF1F130}" name="offline / online" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -425,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -456,20 +458,56 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>45785</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.85416666666666663</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <f>Table1[[#This Row],[To]]-Table1[[#This Row],[From]]</f>
         <v>6.25E-2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>45788</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Table1[[#This Row],[To]]-Table1[[#This Row],[From]]</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>45792</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Table1[[#This Row],[To]]-Table1[[#This Row],[From]]</f>
+        <v>0.14583333333333326</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>